<commit_message>
agregando ajustes de boostrap, modal de alerta y presentacion de errores
</commit_message>
<xml_diff>
--- a/avisos.xlsx
+++ b/avisos.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -419,9 +419,26 @@
         <v>Estado</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>AURICULAR</v>
+      </c>
+      <c r="B2" t="str">
+        <v>b3535</v>
+      </c>
+      <c r="C2" t="str">
+        <v>pablo</v>
+      </c>
+      <c r="D2" t="str">
+        <v>2494381023</v>
+      </c>
+      <c r="E2" t="str">
+        <v>Avisado</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>